<commit_message>
Added support for LINUX
</commit_message>
<xml_diff>
--- a/Datasets/RawDatasets/Vendite.xlsx
+++ b/Datasets/RawDatasets/Vendite.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcovinciguerra/Github/SCGProject/Datasets/RawDatasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2C7F12-8571-B848-9211-FE9D2252D639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094DBD5D-D4BF-E04E-B354-2BE51514A915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1399,9 +1399,6 @@
     <t>CONSUNTIVO</t>
   </si>
   <si>
-    <t>budget/cons</t>
-  </si>
-  <si>
     <t>TipoMovimento</t>
   </si>
   <si>
@@ -1421,6 +1418,9 @@
   </si>
   <si>
     <t>ImportoVenditaInValutaLocaleTOTALEVENDITA</t>
+  </si>
+  <si>
+    <t>budgetCons</t>
   </si>
 </sst>
 </file>
@@ -1872,28 +1872,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>455</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>456</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>457</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>458</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>459</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>461</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>